<commit_message>
data ajustes y chatbot
</commit_message>
<xml_diff>
--- a/data/Anomalias Robos P&G.xlsx
+++ b/data/Anomalias Robos P&G.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ilspglobalsegu-my.sharepoint.com/personal/erivas_ai27_com/Documents/Documentos/Areas de Trabajo/Inteligencia de Negocios/Aplicaciones/App PG/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ilspglobalsegu-my.sharepoint.com/personal/erivas_ai27_com/Documents/Documentos/Areas de Trabajo/Inteligencia de Negocios/Aplicaciones/Productivo/RiesgoPG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{F96B09EB-0188-4BD2-A735-86C26D0F4600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6360B759-ABA8-441C-8C0E-8F158FAF064E}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{F96B09EB-0188-4BD2-A735-86C26D0F4600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE8E54FD-11C4-4F04-912E-DC74D897988A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{182C3EFE-21F3-454B-A9ED-9F81719E5517}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6482" uniqueCount="1218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6796" uniqueCount="1283">
   <si>
     <t>TC 1804 COMPARTE EVIDENCIAS DE UNIDAD EN PENSION POR REPORTE DE  LT  EN ESPERA DE ENTREGA CON CTE
 36AF8L
@@ -6383,6 +6383,201 @@
   <si>
     <t>Bitácora</t>
   </si>
+  <si>
+    <t>MISAEL BALDERAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDAD DETENIDA EN CIRCUITO EXTERIOR MEXIQUENSE A LA ALTURA DE  JARDINES DE SAN MARCOS, EN ESPERA DE REINICIO DE VIAJE. OP NO RESPONDE LLAMADAS. SE PIDE PDM A LT. ENT. SUP, LIZ  🦄LAHM🦄  J65   08/08/2023 07:28   CTO EXTERIOR MEXIQUENSE 1833, 56643 MÉX., MÉXICO   UNIDAD ENCENDIDA   00:00 HH:MM   0 KM/H   19.301054, -98.874623   ACTIVO   ACTIVO </t>
+  </si>
+  <si>
+    <t>AGUSTIN HERNÁNDEZ CORTÉS</t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA EN KM 83 DE COSAMALOAPAN - ACAYUCAN, ESTADÍA POR FALLA MECANICA, COMENTA LO ESTA ARREGLANDO CON EL ECO J48 Y REINICIAN EN POCO TIEMPO. OP CONFIRMA CLAVE DE AMAGO. SE LE SUGIERE PDM ENT. SUP, LIZ  🦄LAHM🦄  J65   08/08/2023 18:20   AMOZOC DE MOTA - NOGALES 870, 75158 PUE., MÉXICO   UNIDAD APAGADA   00:00 HH:MM   0 KM/H   18.332647, -95.818948   INACTIVO   ACTIVO</t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA EN KM 83 DE COSAMALOAPAN - ACAYUCAN, ESTADÍA POR FALLA MECANICA, COMENTA LO ESTA ARREGLANDO CON EL ECO J48 Y REINICIAN EN POCO TIEMPO.OP CONFIRMA CLAVE DE AMAGO.SE LE SUGIERE PDMENT. SUP, LIZ  🦄LAHM🦄  J65  08/08/2023 18:20  AMOZOC DE MOTA - NOGALES 870, 75158 PUE., MÉXICO  UNIDAD APAGADA   00:00 HH:MM  0 KM/H   18.332647, -95.818948  INACTIVO   ACTIVO</t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA EN  E: CARRETERA VILLAHERMOSA-FRONTERA COLONIA: MUNICIPIO: CENTLA ESTADO: TAB   OP DA  CLAVE DE AMAGO SE DETIENE POR UN CAFE LFMH  J65   09/08/2023 03:52   CARR. CTO. DEL GOLFO 96A, PUEBLO NUEVO, 86560 HEROICA CÁRDENAS, TAB., MÉXICO   UNIDAD APAGADA   00:00 HH:MM   0 KM/H   18.523504, -92.638383   INACTIVO   ACTIVO</t>
+  </si>
+  <si>
+    <t>DABRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALFREDO MARTINEZ </t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA SOBRE CARRETERA XALAPA PASO DE OVEJAS, EMILIANO ZAPATA VER;   OPERADOR CONFIRMA CLAVE DE AMAGO; EN ESTADÍA HASTA LA 10 P.M PARA CONTINIAR CON RECORRIDO; SE SOLICITA PARO DE MOTOR A LT; SE NOTIFICA A SUPERVISOR EN TURNO; GPM***   MOVIL ST7171 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 80% FECHA/HORA: 2023/08/09 21:13:55 UBICACIÓN:19.393372, -96.618795 VELOCIDAD:0 KM/H CALLE: CARRETERA XALAPA PASO DE OVEJAS COLONIA: MUNICIPIO: EMILIANO ZAPATA ESTADO: VER</t>
+  </si>
+  <si>
+    <t>GPS NO ACTUALIZA</t>
+  </si>
+  <si>
+    <t>UNIDAD EN RECORRIDO EN  CARRETERA CALPULALPAN-APIZACO OP  CONFIRMA CLAVE DE AMAGO   SE VIZUALIZA  POR C-E  UNIDAD EN RECORRIDO  AACC UBICACIÓN: 19.451074, -98.257667 CALLE:  COLONIA: MUNICIPIO: XALTOCAN ESTADO: TLAX CP.:</t>
+  </si>
+  <si>
+    <t>LT NO RESPONDE NI OPERADOR  MOVIL: MOVIL ST7171 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 80% FECHA/HORA: 2023/08/10 06:37:19 UBICACIÓN: 19.966546, -99.039061 VELOCIDAD: 0 KM/H CALLE: CALLE FRANCISCO I. MADERO COLONIA: SANTA MARÍA AJOLOAPAN MUNICIPIO: HUEYPOXTLA ESTADO: EDOMEX CP.: 55679</t>
+  </si>
+  <si>
+    <t>LEONARDO CORCETTI</t>
+  </si>
+  <si>
+    <t>TERMINAL PANTACO</t>
+  </si>
+  <si>
+    <t>AV DE LOS MAESTROS, SAN ANDRES ATENCO, TLALNEPANTLA, UNIDAD EN ESTADIA CON GRUA POR FALLA MECANICA DE ESTA, EN ESPERA DE REINCIIO HACIA CORRALON-----MOVIL: MOVIL ST7650 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 50% FECHA/HORA: 2023/08/14 23:01:30 UBICACIÓN:19.540328, -99.218642 VELOCIDAD:0 KM/H CALLE: AVENIDA DE LOS MAESTROS COLONIA: SAN ANDRÉS ATENCO AMPLIACIÓN MUNICIPIO: TLALNEPANTLA DE BAZ ESTADO: EDOMEX CP.: 54040</t>
+  </si>
+  <si>
+    <t>EFREN QUINTERO</t>
+  </si>
+  <si>
+    <t>UNIDAD SE VISUALIZA DETENIDO EN KM 150 PARADOR SAN PEDRO   MCSM*-* OP CONFIRMA CLAVE  REPORTA ESTADIA POR DESCANSO  SE LE SUGIERE PARO DE MOTOR  REINICIA A LAS 5:00AM APROX  002377 CLAVE 60AE4M PLACAS -99.931421 LONGITUD     VOLVO MARCA 2009 MODELO 20.31578 LATITUD 4V4NC9TG79N279185 N. DE SERIE 79350180 N. DE MOTOR 2023-08-14 23:03:33 ULTIMA</t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA EN FISCALIA DE ATIZAPAN-----MOVIL: MOVIL ST7650 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 50% FECHA/HORA: 2023/08/15 02:47:25 UBICACIÓN:19.543630, -99.234757 VELOCIDAD:0 KM/H CALLE: BOULEVARD ADOLFO LÓPEZ MATEOS COLONIA: EL POTRERO MUNICIPIO: CIUDAD LÓPEZ MATEOS ESTADO: EDOMEX CP.: 52975</t>
+  </si>
+  <si>
+    <t>UNIDAD SE VISUALIZA EN PENSION SOBRE TLALNEPANTLA DE BAZ  MCSM*-* OP NO ATIENDE MEDIO  EN ESPERA DE MAS INFORMACION POR PARTE DE LT  ENTERADA LIZ   : MOVIL ST7650 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 40% FECHA/HORA: 2023/08/16 01:21:07 UBICACIÓN: 19.584635, -99.200625 VELOCIDAD: 0 KM/H CALLE: ANDADOR DEL GAS COLONIA: SAN PEDRO BARRIENTOS MUNICIPIO: TLALNEPANTLA DE BAZ ESTADO: EDOMEX CP.: 54010</t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA EN JIMENEZ-TORREON KM 129// OPNO CONTESTA MEDIO// SE SOLICITA ESTATUS A LT// LRT//60AE4M PLACAS -104.058924 LONGITUD     VOLVO MARCA 2009 MODELO 26.58799 LATITUD 4V4NC9TG79N279185 N. DE SERIE 79350180 N. DE MOTOR 2023-08-16 04:16:32 ULTIMA TORREON-JIMÉNEZ, RANCHO EL ALTO, DURANGO, MÉXICO</t>
+  </si>
+  <si>
+    <t>MAURO TREJO NAVA</t>
+  </si>
+  <si>
+    <t>UNIDAD  DETENIDA EN KM 87  TEPOTZOTLAN  - PALMILLAS    OP.  TOMA LLAMADA PERO HAY MUCHOA ONTERFERENCIA SE MARCA POR MEDIO TC 7364 Y NO CONTESTA   VGA    MOVIL C9314 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 52% FECHA/HORA: 2023/08/25 19:59:38 UBICACIÓN: 19.993352, -99.471780 VELOCIDAD: 0 KM/H CALLE: MEX-57D COLONIA: MUNICIPIO: SOYANIQUILPAN DE JUÁREZ ESTADO: EDOMEX CP.:</t>
+  </si>
+  <si>
+    <t>PASANDO CASETA SLP., SIN CONTATO CON OPERADOR NI LT  722 830 8836, SE SOLICITA ESTATUS Y PARO DE MOTOR VIA WA---MOVIL: MOVIL C9314 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 43.3% FECHA/HORA: 2023/08/26 01:57:05 UBICACIÓN:22.134657, -100.825922 VELOCIDAD:1 KM/H CALLE: MEX-57D COLONIA: MUNICIPIO: SAN LUIS POTOSÍ ESTADO: SLP CP.:</t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA EN KM 11, SOBRE SLP- MATEHUALA  OP NO CONTESTA LLAMADA, ENETERADO SUPER EN LINEA   LFAI   UBICACIÓN: 22.134697, -100.825891 CALLE: MEX-57D MUNICIPIO: SAN LUIS POTOSÍ ESTADO: SLP</t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA EN KM 21 DE MTY- LA CARBONERA , EN ESPERA DE REINICIO, ,  POR LT EN ALIMENTOS,  COMENTARIO ANTERIOR, IER  MOVIL C9314 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 40% FECHA/HORA: 2023/08/26 13:34:20 UBICACIÓN: 25.593504, -100.879084 VELOCIDAD: 0 KM/H MUNICIPIO: RAMOS ARIZPE ESTADO: COAH</t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA EN ESPERA DE MAS INFORMACIÓN POR PARTE DE LT  © JADG ©  DESCRIPCIÓNECO 06 // 275EX5 // VOLVOPLACA / PATENTE275AX5MARCAUNKNOWN MAKEMODELOUNKNOWN MODELUBICACIÓNMUNICIPIO DE VERACRUZ, VERACRUZ DE IGNACIO DE LA LLAVE, MÉXICO ESTADÍSTICAS0VIAJES0.0KMDISTANCIA0H0M0SDURACIÓN</t>
+  </si>
+  <si>
+    <t>ERIK GONZALEZ PLATA</t>
+  </si>
+  <si>
+    <t>TEPOTZOTLAN-PALMILLAS KM 143, SIN CONTACTO CON OPERADOR, LT 56 1500 1316 REPORTA ESTADIA POR COMPRA DE CIGARROS Y USO DE SANITARIO, SE SOLICITA PARO DE MOTOR----MOVIL ST7191GPS_FIXEDDATE_RANGE 20.277952, -99.890932 FILE_COPY 90.00 % BATTERY_FULL 0 KM/H 2023/08/29 21:33:25</t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDAD EN  EL  KM  458  SOBRE  ZINAPECUARO  --  GUADALAJARA  OP  CINFI9RMA CLAVE DE AMAGO   SE DETUVO  UN MOMENTO  PARA CHECAR LA DIRECCION   DE SU  DESTINO   RETOMA  10  MINUTOS  SE LE SUGIRE   PDM AACC MOVIL: MOVIL ST7191 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 90% FECHA/HORA: 2023/08/30 03:54:56 UBICACIÓN:20.527410, -103.003783 VELOCIDAD:0 KM/H CALLE: MEX-15D COLONIA: MUNICIPIO: ZAPOTLANEJO ESTADO: JAL CP.:</t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDAD EN  ZINAPECUARO  --GUADALAJARA   PASANDO  LA CASETA DE LA  JOYA   OP  CONFIRMA CLAVE DE AMAGO   COMENTA QUE SE DETUVO  POR LE APAGARON SU UNIDAD  QUE  LO CHECARA  CON MONITOREO   AACC MOVIL: MOVIL ST7191 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 80% FECHA/HORA: 2023/08/30 04:33:23 UBICACIÓN:20.603782, -103.141378 VELOCIDAD:0 KM/H CALLE: MEX-90D COLONIA: MUNICIPIO: ZAPOTLANEJO ESTADO: JAL CP.:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASCUAL ORTEGA </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UNIDAD EN ORIGEN EN ESPERA DE INICIO DE VIAJE **AACC*$  MOVIL: MOVIL S2279 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 100% FECHA/HORA: 2023/09/12 22:09:57 UBICACIÓN: 19.608423, -99.222567 VELOCIDAD: 0 KM/H CALLE: AVENIDA TEJOCOTES COLONIA: PARQUE INDUSTRIAL SAN MARTÍN OBISPO MUNICIPIO: CUAUTITLÁN IZCALLI ESTADO: EDOMEX CP.: 54769</t>
+  </si>
+  <si>
+    <t>TEPOTZOTLAN-PALMILLAS KM 106, SIN CONTACTO CON OPERADOR, DHL REFIERE EN BREVE PROPORCIONA ESTATUS, SE SOLICITA PARO DE MOTOR Y EVIDENCIA---MOVIL: MOVIL S2279 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 0% FECHA/HORA: 2023/09/13 02:19:22 UBICACIÓN:20.082931, -99.625844 VELOCIDAD:0 KM/H CALLE: MEX-57D COLONIA: MUNICIPIO: JILOTEPEC ESTADO: EDOMEX CP.:</t>
+  </si>
+  <si>
+    <t>FRANSICO SILVERIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TULTITLAN EDOMEX - CEDIS SORIANA </t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA EN  CARRETERA CUAUTITLÁN-TLALNEPANTLA A LA ALTIUURA DE TULTITLÁN ESTADO: EDOMEX  OP NO RESPONDE LLAMADA, ENETERADO SUPER EN TURNO   LFAI  E-802 FRANCISCO SILVERIO DIRECCION:  POSICION: 19.633375 °, -99.184398 ° ALTITUD: 0 M ANGULO: 74 ° VELOCIDAD: 0 KPH HORA: 2023-09-19 04:38:23</t>
+  </si>
+  <si>
+    <t>ARTURO CAMACHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDAD SE VISUALIZA DETENIDA EN  AVENIDA SAN ANTONIO COLONIA: ANTORCHISTA MARGARITA MORÁN VÉLEZ MUNICIPIO: SAN MARTÍN TEXMELUCAN ESTADO: PUE EN ESPERA DE MAS INF.   VGA   11AX6H HACE 2 MIN 55 S (19.09.2023 07:53:03) AVENIDA SAN ANTONIO, ANTORCHISTA MARGARITA MORÁN VÉLEZ, SAN MARTÍN TEXMELUCAN, PUEBLA 74030, MEXICO 0 KM/H 110287 KM 64.28 H 22 19.301903 -98.426203 </t>
+  </si>
+  <si>
+    <t>LINEAS UNIDAS ZACATECANAS</t>
+  </si>
+  <si>
+    <t>EDGAR BERCOVICH LOPEZ</t>
+  </si>
+  <si>
+    <t>OPERADORA FUTURAMA CIUDAD JUAREZ</t>
+  </si>
+  <si>
+    <t>OP NO RESPONDE LLAMADA SE INFORMA A SUP EN TURNO DETENIDO SOBRE LIBRAMIENTO NORTE SAN LUIS POTOSÍ MUNICIPIO: SOLEDAD DE GRACIANO SÁNCHEZ ESTADO: SLP FBMM HTTPS://WWW.GOOGLE.COM/MAPS?LL=22.266963,-100.870572&amp;Z=15&amp;T=M&amp;HL=EN&amp;GL=US&amp;MAPCLIENT=APIV3</t>
+  </si>
+  <si>
+    <t>UNIDAD EN ESPERA DEL REINICIO DE RECORRIDO  HTTPS://WWW.GOOGLE.COM/MAPS?LL=22.301165,-100.968725&amp;Z=19&amp;T=M&amp;HL=EN&amp;GL=US&amp;MAPCLIENT=APIV3</t>
+  </si>
+  <si>
+    <t>7A5181787</t>
+  </si>
+  <si>
+    <t>TRANSPORTES TORRES TERRESTRES</t>
+  </si>
+  <si>
+    <t>JOSE ISIDRO VELAZQUEZ</t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA EN KM 120 SAN JUAN DE LOS LAGOS DE JAL OP BRINDA PLACAS POR QUE NO RECUERDA SU CLAVE DE AMAGO Y ESTADÍA POR ALIMENTOS SE LE SUGIERE PARO DE MOTOR. ENT. SUP. LILI.  ♥LAHM♥  2023/10/05 05:27:03 PM DIRECCIÓN: AUTOPISTA LAGOS DE MORENO - ZAPOTLANEJO, AGUA DE OBISPO, SAN JUAN DE LOS LAGOS, JALISCO, MÉXICO LATITUD: 21.289074 LONGITUD: -102.240763 ALTITUD: 0 DURACIÓN: HRS</t>
+  </si>
+  <si>
+    <t>7A5225719</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
+  <si>
+    <t>JUAN CARLOS COSME VAZQUEZ</t>
+  </si>
+  <si>
+    <t>AG VILLAHERMOSA</t>
+  </si>
+  <si>
+    <t>UNIDAD EN RESGUARDO EN ESPERA DE INICIO DE RECORRIDO  *F2  CONFIRMA  UNIDAD INGRESA A CORRALON* SE CONFIRMA POR CE ST ENTERADO   NHAF  153ED3 (T-117) EN 18/10/2023 0 KM/H A LAS 17:54 H (UTC - 6) ODÓMETRO : 320.542,2 KM DISESUR • BAJA CALIFORNIA, 3202, MÉXICO, TEHUACÁN, PUE., MÉXICO, 75764 18.455187, -97.414499</t>
+  </si>
+  <si>
+    <t>7A5239262</t>
+  </si>
+  <si>
+    <t>SAGOT</t>
+  </si>
+  <si>
+    <t>HILARIO JESUS NIETO JUAREZ</t>
+  </si>
+  <si>
+    <t>UNIDAD EN RUTA EN KM 3 DE IRAPUATO-SALAMANCA OP BRINDA PLACAS Y DESTINO, NO RECUERDA SU CLAVE. DESVIO DE RUTA. ENT SUP LIZ  ♥LAHM♥  MOVIL: MOVIL ST8488 TIPO DE GPS: REMOLQUE NIVEL DE BATERÍA: 100% FECHA/HORA: 2023/10/25 09:54:38 UBICACIÓN: 20.683913, -101.304438 VELOCIDAD: 74 KM/H CALLE: MEX-45 COLONIA: MUNICIPIO: IRAPUATO ESTADO: GTO CP.:</t>
+  </si>
+  <si>
+    <t>7A5239332</t>
+  </si>
+  <si>
+    <t>SERGIO MERAZ LOPEZ</t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA EN KM.275 DE ESPERANZA-FORTIN OP CONFIRMA AMAGO Y MENCIONA QUE EL TRÁFICO ESTÁ TOTALMENTE PARADO//SE CORROBORA POR GMAPS AJAA ---  57AG2R  PLACAS SIN PLACAS V.PRINCIPAL 13.92 V BATERIA 4.08 V ODOMETRO 1,981,370.74 KM (C) TEMPETARURA 0 ºC LAT / LON 18.85030660 / -97.07032660 UBICACIÓN AUTOPISTA 725, AUTOPISTA, 94340 ORIZABA, VER., MEXICO</t>
+  </si>
+  <si>
+    <t>7A5241021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUIS ANGEL SANCHEZ </t>
+  </si>
+  <si>
+    <t>CEDIS OXXO OBREGON SONORA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUT MEX-QRO A LA ALTURA DE LA DIXON, OPERADOR REPORTA ESTADIA EN ESPERA DE CONVOY, CONFIRMA CCLAVE, SE SUGIERE SOLICITE PARO DE MOTOR--- TORO LUIS ANGEL 37BA4R TRANSPORTES DEL TORO 25/10 20:11 </t>
+  </si>
+  <si>
+    <t>UNIDAD DETENIDA EN DOS BOCAS COLONIA: MUNICIPIO: CUNDUACÁN ESTADO: TAB OP NO ATIENDE MEDIO//ENTERADA SUP. LILY//SE MANTIENE AJAA   57AG2R  PLACAS SIN PLACAS V.PRINCIPAL 13.86 V BATERIA 4.08 V ODOMETRO 1,981,836.81 KM (C) TEMPETARURA 0 ºC LAT / LON 17.99164500 / -93.13246160 UBICACIÓN REFORMA - DOS BOCAS, TABASCO, MEXICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDAD DETENIDA EN REFORMA DOS BOCAS, TAB SE PIDE ESTATUS A LT SE CONFIRMA POR CE ST ENTERADO   NHAF   57AG2R (UNIDAD DETENIDA) EN ESTADO ODÓMETRO CURSO COMBUSTIBLE 39 MINUTOS 1981838 KM  306.6° 123.53 L 2023-10-26 08:49 18.012036, -93.144131     </t>
+  </si>
 </sst>
 </file>
 
@@ -6410,11 +6605,31 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -6424,7 +6639,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6464,6 +6679,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6781,13 +7006,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB9DB00-C084-4852-8E5D-982FCA460831}">
-  <dimension ref="A1:P661"/>
+  <dimension ref="A1:P695"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A667" workbookViewId="0">
+      <selection activeCell="K679" sqref="K679"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
@@ -39833,6 +40061,1706 @@
         <v>0</v>
       </c>
     </row>
+    <row r="662" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A662" s="14">
+        <v>785023514</v>
+      </c>
+      <c r="B662" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C662" s="16">
+        <v>17294631</v>
+      </c>
+      <c r="D662" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E662" s="15" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F662" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G662" t="s">
+        <v>4</v>
+      </c>
+      <c r="H662" s="15" t="s">
+        <v>665</v>
+      </c>
+      <c r="I662" t="s">
+        <v>50</v>
+      </c>
+      <c r="J662" s="2">
+        <v>1379</v>
+      </c>
+      <c r="K662" s="2">
+        <v>24</v>
+      </c>
+      <c r="L662" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M662" s="15">
+        <v>19.301054000000001</v>
+      </c>
+      <c r="N662" s="15">
+        <v>-98.874623</v>
+      </c>
+      <c r="O662" s="17">
+        <v>45146.313691435185</v>
+      </c>
+      <c r="P662" s="15" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="663" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A663" s="14">
+        <v>785023514</v>
+      </c>
+      <c r="B663" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C663" s="16">
+        <v>17294631</v>
+      </c>
+      <c r="D663" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E663" s="15" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F663" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G663" t="s">
+        <v>4</v>
+      </c>
+      <c r="H663" s="15" t="s">
+        <v>665</v>
+      </c>
+      <c r="I663" t="s">
+        <v>50</v>
+      </c>
+      <c r="J663" s="2">
+        <v>1379</v>
+      </c>
+      <c r="K663" s="2">
+        <v>24</v>
+      </c>
+      <c r="L663" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M663" s="15">
+        <v>18.332647000000001</v>
+      </c>
+      <c r="N663" s="15">
+        <v>-95.818948000000006</v>
+      </c>
+      <c r="O663" s="17">
+        <v>45146.770613043984</v>
+      </c>
+      <c r="P663" s="15" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="664" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A664" s="14">
+        <v>785023514</v>
+      </c>
+      <c r="B664" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C664" s="16">
+        <v>17294631</v>
+      </c>
+      <c r="D664" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E664" s="15" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F664" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G664" t="s">
+        <v>4</v>
+      </c>
+      <c r="H664" s="15" t="s">
+        <v>665</v>
+      </c>
+      <c r="I664" t="s">
+        <v>50</v>
+      </c>
+      <c r="J664" s="2">
+        <v>1379</v>
+      </c>
+      <c r="K664" s="2">
+        <v>24</v>
+      </c>
+      <c r="L664" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M664" s="15">
+        <v>18.332647000000001</v>
+      </c>
+      <c r="N664" s="15">
+        <v>-95.818948000000006</v>
+      </c>
+      <c r="O664" s="17">
+        <v>45146.77102954861</v>
+      </c>
+      <c r="P664" s="15" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="665" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A665" s="14">
+        <v>785023514</v>
+      </c>
+      <c r="B665" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C665" s="16">
+        <v>17294631</v>
+      </c>
+      <c r="D665" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E665" s="15" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F665" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G665" t="s">
+        <v>4</v>
+      </c>
+      <c r="H665" s="15" t="s">
+        <v>665</v>
+      </c>
+      <c r="I665" t="s">
+        <v>50</v>
+      </c>
+      <c r="J665" s="2">
+        <v>1379</v>
+      </c>
+      <c r="K665" s="2">
+        <v>24</v>
+      </c>
+      <c r="L665" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M665" s="15">
+        <v>18.523503999999999</v>
+      </c>
+      <c r="N665" s="15">
+        <v>-92.638383000000005</v>
+      </c>
+      <c r="O665" s="17">
+        <v>45147.164623460645</v>
+      </c>
+      <c r="P665" s="15" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="666" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A666" s="14">
+        <v>785028330</v>
+      </c>
+      <c r="B666" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C666" s="16">
+        <v>4507118446</v>
+      </c>
+      <c r="D666" s="15" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E666" s="15" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F666" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G666" t="s">
+        <v>2</v>
+      </c>
+      <c r="H666" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="I666" t="s">
+        <v>114</v>
+      </c>
+      <c r="J666" s="2">
+        <v>1262</v>
+      </c>
+      <c r="K666" s="2">
+        <v>11</v>
+      </c>
+      <c r="L666" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M666" s="15">
+        <v>19.393371999999999</v>
+      </c>
+      <c r="N666" s="15">
+        <v>-96.618795000000006</v>
+      </c>
+      <c r="O666" s="17">
+        <v>45147.844227893518</v>
+      </c>
+      <c r="P666" s="15" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="667" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A667" s="14">
+        <v>785028330</v>
+      </c>
+      <c r="B667" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C667" s="16">
+        <v>4507118446</v>
+      </c>
+      <c r="D667" s="15" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E667" s="15" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F667" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G667" t="s">
+        <v>2</v>
+      </c>
+      <c r="H667" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="I667" t="s">
+        <v>114</v>
+      </c>
+      <c r="J667" s="2">
+        <v>1262</v>
+      </c>
+      <c r="K667" s="2">
+        <v>11</v>
+      </c>
+      <c r="L667" s="15" t="s">
+        <v>1227</v>
+      </c>
+      <c r="M667" s="15">
+        <v>19.451073999999998</v>
+      </c>
+      <c r="N667" s="15">
+        <v>-98.257666999999998</v>
+      </c>
+      <c r="O667" s="17">
+        <v>45148.094911840279</v>
+      </c>
+      <c r="P667" s="15" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="668" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A668" s="14">
+        <v>785028330</v>
+      </c>
+      <c r="B668" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C668" s="16">
+        <v>4507118446</v>
+      </c>
+      <c r="D668" s="15" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E668" s="15" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F668" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G668" t="s">
+        <v>2</v>
+      </c>
+      <c r="H668" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="I668" t="s">
+        <v>114</v>
+      </c>
+      <c r="J668" s="2">
+        <v>1262</v>
+      </c>
+      <c r="K668" s="2">
+        <v>11</v>
+      </c>
+      <c r="L668" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M668" s="15">
+        <v>19.966546000000001</v>
+      </c>
+      <c r="N668" s="15">
+        <v>-99.039061000000004</v>
+      </c>
+      <c r="O668" s="17">
+        <v>45148.28073017361</v>
+      </c>
+      <c r="P668" s="15" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="669" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A669" s="14">
+        <v>785040571</v>
+      </c>
+      <c r="B669" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C669" s="16">
+        <v>1417604770</v>
+      </c>
+      <c r="D669" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="E669" s="15" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F669" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G669" t="s">
+        <v>4</v>
+      </c>
+      <c r="H669" s="15" t="s">
+        <v>1231</v>
+      </c>
+      <c r="I669" t="s">
+        <v>197</v>
+      </c>
+      <c r="J669" s="2">
+        <v>69</v>
+      </c>
+      <c r="K669" s="2">
+        <v>2</v>
+      </c>
+      <c r="L669" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M669" s="15">
+        <v>19.540327999999999</v>
+      </c>
+      <c r="N669" s="15">
+        <v>-99.218642000000003</v>
+      </c>
+      <c r="O669" s="17">
+        <v>45152.96019366898</v>
+      </c>
+      <c r="P669" s="15" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="670" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A670" s="14">
+        <v>785041068</v>
+      </c>
+      <c r="B670" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C670" s="16">
+        <v>17297763</v>
+      </c>
+      <c r="D670" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="E670" s="15" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F670" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G670" t="s">
+        <v>4</v>
+      </c>
+      <c r="H670" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="I670" t="s">
+        <v>4</v>
+      </c>
+      <c r="J670" s="2">
+        <v>100</v>
+      </c>
+      <c r="K670" s="2">
+        <v>2</v>
+      </c>
+      <c r="L670" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M670" s="15">
+        <v>20.31578</v>
+      </c>
+      <c r="N670" s="15">
+        <v>-99.931421</v>
+      </c>
+      <c r="O670" s="17">
+        <v>45152.967815046293</v>
+      </c>
+      <c r="P670" s="15" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="671" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A671" s="14">
+        <v>785040571</v>
+      </c>
+      <c r="B671" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C671" s="16">
+        <v>1417604770</v>
+      </c>
+      <c r="D671" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="E671" s="15" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F671" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G671" t="s">
+        <v>4</v>
+      </c>
+      <c r="H671" s="15" t="s">
+        <v>1231</v>
+      </c>
+      <c r="I671" t="s">
+        <v>197</v>
+      </c>
+      <c r="J671" s="2">
+        <v>69</v>
+      </c>
+      <c r="K671" s="2">
+        <v>2</v>
+      </c>
+      <c r="L671" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M671" s="15">
+        <v>19.54363</v>
+      </c>
+      <c r="N671" s="15">
+        <v>-99.234757000000002</v>
+      </c>
+      <c r="O671" s="17">
+        <v>45153.116454513889</v>
+      </c>
+      <c r="P671" s="15" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="672" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A672" s="14">
+        <v>785040571</v>
+      </c>
+      <c r="B672" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C672" s="16">
+        <v>1417604770</v>
+      </c>
+      <c r="D672" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="E672" s="15" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F672" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G672" t="s">
+        <v>4</v>
+      </c>
+      <c r="H672" s="15" t="s">
+        <v>1231</v>
+      </c>
+      <c r="I672" t="s">
+        <v>197</v>
+      </c>
+      <c r="J672" s="2">
+        <v>69</v>
+      </c>
+      <c r="K672" s="2">
+        <v>2</v>
+      </c>
+      <c r="L672" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M672" s="15">
+        <v>19.584634999999999</v>
+      </c>
+      <c r="N672" s="15">
+        <v>-99.200625000000002</v>
+      </c>
+      <c r="O672" s="17">
+        <v>45154.060072453707</v>
+      </c>
+      <c r="P672" s="15" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="673" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A673" s="14">
+        <v>785041068</v>
+      </c>
+      <c r="B673" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C673" s="16">
+        <v>17297763</v>
+      </c>
+      <c r="D673" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="E673" s="15" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F673" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G673" t="s">
+        <v>4</v>
+      </c>
+      <c r="H673" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="I673" t="s">
+        <v>4</v>
+      </c>
+      <c r="J673" s="2">
+        <v>100</v>
+      </c>
+      <c r="K673" s="2">
+        <v>2</v>
+      </c>
+      <c r="L673" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M673" s="15">
+        <v>26.587990000000001</v>
+      </c>
+      <c r="N673" s="15">
+        <v>-104.058924</v>
+      </c>
+      <c r="O673" s="17">
+        <v>45154.182606481481</v>
+      </c>
+      <c r="P673" s="15" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="674" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A674" s="14">
+        <v>785071453</v>
+      </c>
+      <c r="B674" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C674" s="16">
+        <v>1417632985</v>
+      </c>
+      <c r="D674" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="E674" s="15" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F674" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G674" t="s">
+        <v>197</v>
+      </c>
+      <c r="H674" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I674" t="s">
+        <v>24</v>
+      </c>
+      <c r="J674" s="2">
+        <v>752</v>
+      </c>
+      <c r="K674" s="2">
+        <v>11</v>
+      </c>
+      <c r="L674" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M674" s="15">
+        <v>19.993352000000002</v>
+      </c>
+      <c r="N674" s="15">
+        <v>-99.471779999999995</v>
+      </c>
+      <c r="O674" s="17">
+        <v>45163.839107210646</v>
+      </c>
+      <c r="P674" s="15" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="675" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A675" s="14">
+        <v>785071453</v>
+      </c>
+      <c r="B675" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C675" s="16">
+        <v>1417632985</v>
+      </c>
+      <c r="D675" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="E675" s="15" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F675" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G675" t="s">
+        <v>197</v>
+      </c>
+      <c r="H675" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I675" t="s">
+        <v>24</v>
+      </c>
+      <c r="J675" s="2">
+        <v>752</v>
+      </c>
+      <c r="K675" s="2">
+        <v>11</v>
+      </c>
+      <c r="L675" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M675" s="15">
+        <v>22.134657000000001</v>
+      </c>
+      <c r="N675" s="15">
+        <v>-100.82592200000001</v>
+      </c>
+      <c r="O675" s="17">
+        <v>45164.08273642361</v>
+      </c>
+      <c r="P675" s="15" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="676" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A676" s="14">
+        <v>785071453</v>
+      </c>
+      <c r="B676" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C676" s="16">
+        <v>1417632985</v>
+      </c>
+      <c r="D676" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="E676" s="15" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F676" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G676" t="s">
+        <v>197</v>
+      </c>
+      <c r="H676" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I676" t="s">
+        <v>24</v>
+      </c>
+      <c r="J676" s="2">
+        <v>752</v>
+      </c>
+      <c r="K676" s="2">
+        <v>11</v>
+      </c>
+      <c r="L676" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M676" s="15">
+        <v>22.134657000000001</v>
+      </c>
+      <c r="N676" s="15">
+        <v>-100.82592200000001</v>
+      </c>
+      <c r="O676" s="17">
+        <v>45164.082864085649</v>
+      </c>
+      <c r="P676" s="15" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="677" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A677" s="14">
+        <v>785071453</v>
+      </c>
+      <c r="B677" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C677" s="16">
+        <v>1417632985</v>
+      </c>
+      <c r="D677" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="E677" s="15" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F677" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G677" t="s">
+        <v>197</v>
+      </c>
+      <c r="H677" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I677" t="s">
+        <v>24</v>
+      </c>
+      <c r="J677" s="2">
+        <v>752</v>
+      </c>
+      <c r="K677" s="2">
+        <v>11</v>
+      </c>
+      <c r="L677" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M677" s="15">
+        <v>22.134696999999999</v>
+      </c>
+      <c r="N677" s="15">
+        <v>-100.825891</v>
+      </c>
+      <c r="O677" s="17">
+        <v>45164.113248530091</v>
+      </c>
+      <c r="P677" s="15" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="678" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A678" s="14">
+        <v>785071453</v>
+      </c>
+      <c r="B678" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C678" s="16">
+        <v>1417632985</v>
+      </c>
+      <c r="D678" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="E678" s="15" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F678" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G678" t="s">
+        <v>197</v>
+      </c>
+      <c r="H678" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I678" t="s">
+        <v>24</v>
+      </c>
+      <c r="J678" s="2">
+        <v>752</v>
+      </c>
+      <c r="K678" s="2">
+        <v>11</v>
+      </c>
+      <c r="L678" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M678" s="15">
+        <v>25.593503999999999</v>
+      </c>
+      <c r="N678" s="15">
+        <v>-100.87908400000001</v>
+      </c>
+      <c r="O678" s="17">
+        <v>45164.569848807871</v>
+      </c>
+      <c r="P678" s="15" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="679" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A679" s="14">
+        <v>785028330</v>
+      </c>
+      <c r="B679" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C679" s="16">
+        <v>4507118446</v>
+      </c>
+      <c r="D679" s="15" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E679" s="15" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F679" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G679" t="s">
+        <v>2</v>
+      </c>
+      <c r="H679" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="I679" t="s">
+        <v>114</v>
+      </c>
+      <c r="J679" s="2">
+        <v>1262</v>
+      </c>
+      <c r="K679" s="2">
+        <v>11</v>
+      </c>
+      <c r="L679" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M679" s="15">
+        <v>19.221035000000001</v>
+      </c>
+      <c r="N679" s="15">
+        <v>-96.191460000000006</v>
+      </c>
+      <c r="O679" s="17">
+        <v>45165.278830243056</v>
+      </c>
+      <c r="P679" s="15" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="680" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A680" s="14">
+        <v>785081715</v>
+      </c>
+      <c r="B680" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C680" s="16">
+        <v>17304626</v>
+      </c>
+      <c r="D680" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E680" s="15" t="s">
+        <v>1244</v>
+      </c>
+      <c r="F680" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G680" t="s">
+        <v>4</v>
+      </c>
+      <c r="H680" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I680" t="s">
+        <v>93</v>
+      </c>
+      <c r="J680" s="2">
+        <v>483</v>
+      </c>
+      <c r="K680" s="2">
+        <v>7</v>
+      </c>
+      <c r="L680" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M680" s="15">
+        <v>20.277908</v>
+      </c>
+      <c r="N680" s="15">
+        <v>-99.890872999999999</v>
+      </c>
+      <c r="O680" s="17">
+        <v>45167.899139004629</v>
+      </c>
+      <c r="P680" s="15" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="681" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A681" s="14">
+        <v>785081715</v>
+      </c>
+      <c r="B681" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C681" s="16">
+        <v>17304626</v>
+      </c>
+      <c r="D681" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E681" s="15" t="s">
+        <v>1244</v>
+      </c>
+      <c r="F681" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G681" t="s">
+        <v>4</v>
+      </c>
+      <c r="H681" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I681" t="s">
+        <v>93</v>
+      </c>
+      <c r="J681" s="2">
+        <v>483</v>
+      </c>
+      <c r="K681" s="2">
+        <v>7</v>
+      </c>
+      <c r="L681" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M681" s="15">
+        <v>20.52741</v>
+      </c>
+      <c r="N681" s="15">
+        <v>-103.003783</v>
+      </c>
+      <c r="O681" s="17">
+        <v>45168.123702974539</v>
+      </c>
+      <c r="P681" s="15" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="682" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A682" s="14">
+        <v>785081715</v>
+      </c>
+      <c r="B682" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C682" s="16">
+        <v>17304626</v>
+      </c>
+      <c r="D682" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E682" s="15" t="s">
+        <v>1244</v>
+      </c>
+      <c r="F682" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G682" t="s">
+        <v>4</v>
+      </c>
+      <c r="H682" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I682" t="s">
+        <v>93</v>
+      </c>
+      <c r="J682" s="2">
+        <v>483</v>
+      </c>
+      <c r="K682" s="2">
+        <v>7</v>
+      </c>
+      <c r="L682" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M682" s="15">
+        <v>20.603781999999999</v>
+      </c>
+      <c r="N682" s="15">
+        <v>-103.141378</v>
+      </c>
+      <c r="O682" s="17">
+        <v>45168.150652314813</v>
+      </c>
+      <c r="P682" s="15" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="683" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A683" s="14">
+        <v>795121704</v>
+      </c>
+      <c r="B683" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C683" s="16">
+        <v>17311025</v>
+      </c>
+      <c r="D683" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E683" s="15" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F683" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G683" t="s">
+        <v>4</v>
+      </c>
+      <c r="H683" s="15" t="s">
+        <v>589</v>
+      </c>
+      <c r="I683" t="s">
+        <v>114</v>
+      </c>
+      <c r="J683" s="2">
+        <v>330</v>
+      </c>
+      <c r="K683" s="2">
+        <v>7</v>
+      </c>
+      <c r="L683" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="M683" s="15">
+        <v>19.608422999999998</v>
+      </c>
+      <c r="N683" s="15">
+        <v>-99.222566999999998</v>
+      </c>
+      <c r="O683" s="17">
+        <v>45181.925582719909</v>
+      </c>
+      <c r="P683" s="15" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="684" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A684" s="14">
+        <v>795121704</v>
+      </c>
+      <c r="B684" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C684" s="16">
+        <v>17311025</v>
+      </c>
+      <c r="D684" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E684" s="15" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F684" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G684" t="s">
+        <v>4</v>
+      </c>
+      <c r="H684" s="15" t="s">
+        <v>589</v>
+      </c>
+      <c r="I684" t="s">
+        <v>114</v>
+      </c>
+      <c r="J684" s="2">
+        <v>330</v>
+      </c>
+      <c r="K684" s="2">
+        <v>7</v>
+      </c>
+      <c r="L684" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M684" s="15">
+        <v>20.082930999999999</v>
+      </c>
+      <c r="N684" s="15">
+        <v>-99.625844000000001</v>
+      </c>
+      <c r="O684" s="17">
+        <v>45182.096898148149</v>
+      </c>
+      <c r="P684" s="15" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="685" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A685" s="14">
+        <v>795136292</v>
+      </c>
+      <c r="B685" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C685" s="16">
+        <v>17314195</v>
+      </c>
+      <c r="D685" s="15" t="s">
+        <v>555</v>
+      </c>
+      <c r="E685" s="15" t="s">
+        <v>1251</v>
+      </c>
+      <c r="F685" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G685" t="s">
+        <v>4</v>
+      </c>
+      <c r="H685" s="15" t="s">
+        <v>1252</v>
+      </c>
+      <c r="I685" t="s">
+        <v>4</v>
+      </c>
+      <c r="J685" s="2">
+        <v>100</v>
+      </c>
+      <c r="K685" s="2">
+        <v>2</v>
+      </c>
+      <c r="L685" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M685" s="15">
+        <v>19.633375000000001</v>
+      </c>
+      <c r="N685" s="15">
+        <v>-99.184398000000002</v>
+      </c>
+      <c r="O685" s="17">
+        <v>45188.201896678242</v>
+      </c>
+      <c r="P685" s="15" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="686" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A686" s="14">
+        <v>795135991</v>
+      </c>
+      <c r="B686" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C686" s="16">
+        <v>17312596</v>
+      </c>
+      <c r="D686" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E686" s="15" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F686" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G686" t="s">
+        <v>4</v>
+      </c>
+      <c r="H686" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="I686" t="s">
+        <v>161</v>
+      </c>
+      <c r="J686" s="2">
+        <v>521</v>
+      </c>
+      <c r="K686" s="2">
+        <v>7</v>
+      </c>
+      <c r="L686" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M686" s="15">
+        <v>19.301902999999999</v>
+      </c>
+      <c r="N686" s="15">
+        <v>-98.426203000000001</v>
+      </c>
+      <c r="O686" s="17">
+        <v>45188.290701122685</v>
+      </c>
+      <c r="P686" s="15" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="687" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A687" s="14">
+        <v>795136773</v>
+      </c>
+      <c r="B687" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C687" s="16">
+        <v>17314654</v>
+      </c>
+      <c r="D687" s="15" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E687" s="15" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F687" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G687" t="s">
+        <v>4</v>
+      </c>
+      <c r="H687" s="15" t="s">
+        <v>1258</v>
+      </c>
+      <c r="I687" t="s">
+        <v>4</v>
+      </c>
+      <c r="J687" s="2">
+        <v>100</v>
+      </c>
+      <c r="K687" s="2">
+        <v>2</v>
+      </c>
+      <c r="L687" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M687" s="15">
+        <v>22.266963000000001</v>
+      </c>
+      <c r="N687" s="15">
+        <v>-100.870572</v>
+      </c>
+      <c r="O687" s="17">
+        <v>45188.684371180556</v>
+      </c>
+      <c r="P687" s="15" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="688" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A688" s="14">
+        <v>795136773</v>
+      </c>
+      <c r="B688" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C688" s="16">
+        <v>17314654</v>
+      </c>
+      <c r="D688" s="15" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E688" s="15" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F688" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G688" t="s">
+        <v>4</v>
+      </c>
+      <c r="H688" s="15" t="s">
+        <v>1258</v>
+      </c>
+      <c r="I688" t="s">
+        <v>4</v>
+      </c>
+      <c r="J688" s="2">
+        <v>100</v>
+      </c>
+      <c r="K688" s="2">
+        <v>2</v>
+      </c>
+      <c r="L688" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M688" s="15">
+        <v>22.301165000000001</v>
+      </c>
+      <c r="N688" s="15">
+        <v>-100.96872500000001</v>
+      </c>
+      <c r="O688" s="17">
+        <v>45188.794248182872</v>
+      </c>
+      <c r="P688" s="15" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="689" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A689" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B689" t="s">
+        <v>9</v>
+      </c>
+      <c r="C689" s="6">
+        <v>17322098</v>
+      </c>
+      <c r="D689" t="s">
+        <v>1262</v>
+      </c>
+      <c r="E689" t="s">
+        <v>1263</v>
+      </c>
+      <c r="F689" t="s">
+        <v>128</v>
+      </c>
+      <c r="G689" t="s">
+        <v>197</v>
+      </c>
+      <c r="H689" t="s">
+        <v>147</v>
+      </c>
+      <c r="I689" t="s">
+        <v>44</v>
+      </c>
+      <c r="J689" s="2">
+        <v>1286</v>
+      </c>
+      <c r="K689" s="2">
+        <v>30</v>
+      </c>
+      <c r="L689" t="s">
+        <v>11</v>
+      </c>
+      <c r="M689">
+        <v>21.289073999999999</v>
+      </c>
+      <c r="N689">
+        <v>-102.240763</v>
+      </c>
+      <c r="O689" s="3">
+        <v>45204.731415162038</v>
+      </c>
+      <c r="P689" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="690" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A690" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B690" t="s">
+        <v>9</v>
+      </c>
+      <c r="C690" s="6" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D690" t="s">
+        <v>164</v>
+      </c>
+      <c r="E690" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F690" t="s">
+        <v>5</v>
+      </c>
+      <c r="G690" t="s">
+        <v>4</v>
+      </c>
+      <c r="H690" t="s">
+        <v>1268</v>
+      </c>
+      <c r="I690" t="s">
+        <v>169</v>
+      </c>
+      <c r="J690" s="2">
+        <v>457</v>
+      </c>
+      <c r="K690" s="2">
+        <v>7</v>
+      </c>
+      <c r="L690" t="s">
+        <v>11</v>
+      </c>
+      <c r="M690">
+        <v>18.455186999999999</v>
+      </c>
+      <c r="N690">
+        <v>-97.414499000000006</v>
+      </c>
+      <c r="O690" s="3">
+        <v>45219.497070057871</v>
+      </c>
+      <c r="P690" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="691" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A691" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B691" t="s">
+        <v>22</v>
+      </c>
+      <c r="C691" s="6">
+        <v>1417712858</v>
+      </c>
+      <c r="D691" t="s">
+        <v>1271</v>
+      </c>
+      <c r="E691" t="s">
+        <v>1272</v>
+      </c>
+      <c r="F691" t="s">
+        <v>205</v>
+      </c>
+      <c r="G691" t="s">
+        <v>114</v>
+      </c>
+      <c r="H691" t="s">
+        <v>132</v>
+      </c>
+      <c r="I691" t="s">
+        <v>24</v>
+      </c>
+      <c r="J691" s="2">
+        <v>1379</v>
+      </c>
+      <c r="K691" s="2">
+        <v>24</v>
+      </c>
+      <c r="L691" t="s">
+        <v>127</v>
+      </c>
+      <c r="M691">
+        <v>20.683913</v>
+      </c>
+      <c r="N691">
+        <v>-101.304438</v>
+      </c>
+      <c r="O691" s="3">
+        <v>45224.373337962963</v>
+      </c>
+      <c r="P691" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="692" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A692" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B692" t="s">
+        <v>9</v>
+      </c>
+      <c r="C692" s="6">
+        <v>17331185</v>
+      </c>
+      <c r="D692" t="s">
+        <v>53</v>
+      </c>
+      <c r="E692" t="s">
+        <v>1275</v>
+      </c>
+      <c r="F692" t="s">
+        <v>5</v>
+      </c>
+      <c r="G692" t="s">
+        <v>4</v>
+      </c>
+      <c r="H692" t="s">
+        <v>1151</v>
+      </c>
+      <c r="I692" t="s">
+        <v>169</v>
+      </c>
+      <c r="J692" s="2">
+        <v>457</v>
+      </c>
+      <c r="K692" s="2">
+        <v>7</v>
+      </c>
+      <c r="L692" t="s">
+        <v>11</v>
+      </c>
+      <c r="M692">
+        <v>18.850307000000001</v>
+      </c>
+      <c r="N692">
+        <v>-97.070327000000006</v>
+      </c>
+      <c r="O692" s="3">
+        <v>45224.819490428243</v>
+      </c>
+      <c r="P692" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="693" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A693" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B693" t="s">
+        <v>9</v>
+      </c>
+      <c r="C693" s="6">
+        <v>17331965</v>
+      </c>
+      <c r="D693" t="s">
+        <v>53</v>
+      </c>
+      <c r="E693" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F693" t="s">
+        <v>5</v>
+      </c>
+      <c r="G693" t="s">
+        <v>4</v>
+      </c>
+      <c r="H693" t="s">
+        <v>1279</v>
+      </c>
+      <c r="I693" t="s">
+        <v>184</v>
+      </c>
+      <c r="J693" s="2">
+        <v>1904</v>
+      </c>
+      <c r="K693" s="2">
+        <v>36</v>
+      </c>
+      <c r="L693" t="s">
+        <v>11</v>
+      </c>
+      <c r="M693">
+        <v>19.611616999999999</v>
+      </c>
+      <c r="N693">
+        <v>-99.189577</v>
+      </c>
+      <c r="O693" s="3">
+        <v>45224.84442627315</v>
+      </c>
+      <c r="P693" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="694" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A694" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B694" t="s">
+        <v>9</v>
+      </c>
+      <c r="C694" s="6">
+        <v>17331185</v>
+      </c>
+      <c r="D694" t="s">
+        <v>53</v>
+      </c>
+      <c r="E694" t="s">
+        <v>1275</v>
+      </c>
+      <c r="F694" t="s">
+        <v>5</v>
+      </c>
+      <c r="G694" t="s">
+        <v>4</v>
+      </c>
+      <c r="H694" t="s">
+        <v>1151</v>
+      </c>
+      <c r="I694" t="s">
+        <v>169</v>
+      </c>
+      <c r="J694" s="2">
+        <v>457</v>
+      </c>
+      <c r="K694" s="2">
+        <v>7</v>
+      </c>
+      <c r="L694" t="s">
+        <v>11</v>
+      </c>
+      <c r="M694">
+        <v>17.991644999999998</v>
+      </c>
+      <c r="N694">
+        <v>-93.132462000000004</v>
+      </c>
+      <c r="O694" s="3">
+        <v>45225.289068518519</v>
+      </c>
+      <c r="P694" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="695" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A695" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B695" t="s">
+        <v>9</v>
+      </c>
+      <c r="C695" s="6">
+        <v>17331185</v>
+      </c>
+      <c r="D695" t="s">
+        <v>53</v>
+      </c>
+      <c r="E695" t="s">
+        <v>1275</v>
+      </c>
+      <c r="F695" t="s">
+        <v>5</v>
+      </c>
+      <c r="G695" t="s">
+        <v>4</v>
+      </c>
+      <c r="H695" t="s">
+        <v>1151</v>
+      </c>
+      <c r="I695" t="s">
+        <v>169</v>
+      </c>
+      <c r="J695" s="2">
+        <v>457</v>
+      </c>
+      <c r="K695" s="2">
+        <v>7</v>
+      </c>
+      <c r="L695" t="s">
+        <v>11</v>
+      </c>
+      <c r="M695">
+        <v>18.012035999999998</v>
+      </c>
+      <c r="N695">
+        <v>-93.144131000000002</v>
+      </c>
+      <c r="O695" s="3">
+        <v>45225.371786689815</v>
+      </c>
+      <c r="P695" t="s">
+        <v>1282</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>